<commit_message>
Add rex bootstrap result and overall results
</commit_message>
<xml_diff>
--- a/results/TGAM/TGAM_bootstrap.xlsx
+++ b/results/TGAM/TGAM_bootstrap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ORnearshore_groundfish\results\TGAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C92045-A079-4FC9-904C-A210E4AA1CE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B92188-B69E-4A3B-915E-BCCA87D807DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Species</t>
   </si>
   <si>
-    <t>Mean</t>
-  </si>
-  <si>
     <t>Arrowtooth</t>
   </si>
   <si>
@@ -60,26 +57,56 @@
     <t>Sablefish</t>
   </si>
   <si>
-    <t>Actual</t>
-  </si>
-  <si>
-    <t>Upper (.95)</t>
-  </si>
-  <si>
-    <t>Lower (.95)</t>
+    <t>Lower (.95) ΔAIC</t>
+  </si>
+  <si>
+    <t>Mean ΔAIC</t>
+  </si>
+  <si>
+    <t>Actual ΔAIC</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Upper (.95) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ΔAIC</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,39 +416,41 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.26953125" customWidth="1"/>
-    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="1" max="2" width="14.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>23.2</v>
@@ -440,7 +470,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>47</v>
@@ -460,7 +490,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>58.44</v>
@@ -480,7 +510,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>125.26</v>
@@ -494,21 +524,33 @@
       <c r="E5">
         <v>200</v>
       </c>
+      <c r="F5" s="1">
+        <v>154.84</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>107.37</v>
+      </c>
+      <c r="C6" s="1">
+        <v>104.37</v>
+      </c>
+      <c r="D6" s="1">
+        <v>105.87</v>
+      </c>
       <c r="E6">
         <v>200</v>
+      </c>
+      <c r="F6" s="1">
+        <v>135.27000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>35.505270000000003</v>
@@ -528,7 +570,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>46.021880000000003</v>
@@ -548,7 +590,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>12.313879999999999</v>
@@ -568,5 +610,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit results of TGAM into dataframe and save boxplot
</commit_message>
<xml_diff>
--- a/results/TGAM/TGAM_bootstrap.xlsx
+++ b/results/TGAM/TGAM_bootstrap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ORnearshore_groundfish\results\TGAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B92188-B69E-4A3B-915E-BCCA87D807DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68741B43-F027-45B8-BA13-0882B5459736}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,65 +27,53 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Arrowtooth</t>
-  </si>
-  <si>
-    <t>Iterations</t>
-  </si>
-  <si>
-    <t>English sole</t>
-  </si>
-  <si>
-    <t>Pacific sanddab</t>
-  </si>
-  <si>
-    <t>Dover sole</t>
-  </si>
-  <si>
-    <t>Rex sole</t>
-  </si>
-  <si>
-    <t>Lingcod</t>
-  </si>
-  <si>
-    <t>Petrale sole</t>
-  </si>
-  <si>
-    <t>Sablefish</t>
-  </si>
-  <si>
-    <t>Lower (.95) ΔAIC</t>
-  </si>
-  <si>
-    <t>Mean ΔAIC</t>
-  </si>
-  <si>
-    <t>Actual ΔAIC</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Upper (.95) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ΔAIC</t>
-    </r>
+    <t>lower_CI</t>
+  </si>
+  <si>
+    <t>upper_CI</t>
+  </si>
+  <si>
+    <t>mean_AIC</t>
+  </si>
+  <si>
+    <t>iterations</t>
+  </si>
+  <si>
+    <t>tgam_AIC</t>
+  </si>
+  <si>
+    <t>arrowtooth</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>sanddab</t>
+  </si>
+  <si>
+    <t>dover</t>
+  </si>
+  <si>
+    <t>species</t>
+  </si>
+  <si>
+    <t>rex</t>
+  </si>
+  <si>
+    <t>lingcod</t>
+  </si>
+  <si>
+    <t>petrale</t>
+  </si>
+  <si>
+    <t>sablefish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,13 +88,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -416,7 +397,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -430,27 +411,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>23.2</v>
@@ -470,7 +451,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>47</v>
@@ -490,7 +471,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>58.44</v>
@@ -510,7 +491,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>125.26</v>
@@ -530,7 +511,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>107.37</v>
@@ -550,7 +531,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>35.505270000000003</v>
@@ -570,7 +551,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>46.021880000000003</v>
@@ -590,7 +571,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>12.313879999999999</v>

</xml_diff>